<commit_message>
Adjusted leaf senescence rate and some phenology for emerald and jade after talking to Neil. Fit for Thomas and Muchow is really good. TOS is going to take some work.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/OldValidationObserved.xlsx
+++ b/Prototypes/Mungbean/OldValidationObserved.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2787BC3C-284F-47A7-9FB9-24B1631041D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C399156-A1D1-468A-A61D-5D755CE0090E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{058C0488-1FD9-4F64-AF6E-B63E9823854A}"/>
   </bookViews>
@@ -826,8 +826,8 @@
   <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4152,7 +4152,7 @@
         <v>809</v>
       </c>
       <c r="H70" s="15">
-        <v>2683</v>
+        <v>268.3</v>
       </c>
       <c r="I70" s="15"/>
       <c r="J70" s="15"/>
@@ -4174,7 +4174,7 @@
         <v>728</v>
       </c>
       <c r="H71" s="15">
-        <v>2435</v>
+        <v>243.5</v>
       </c>
       <c r="I71" s="15"/>
       <c r="J71" s="15"/>
@@ -4196,7 +4196,7 @@
         <v>906</v>
       </c>
       <c r="H72" s="15">
-        <v>2674</v>
+        <v>267.39999999999998</v>
       </c>
       <c r="I72" s="15"/>
       <c r="J72" s="15"/>
@@ -4218,7 +4218,7 @@
         <v>1022</v>
       </c>
       <c r="H73" s="15">
-        <v>2908</v>
+        <v>290.8</v>
       </c>
       <c r="I73" s="15"/>
       <c r="J73" s="15"/>
@@ -4240,7 +4240,7 @@
         <v>1931</v>
       </c>
       <c r="H74" s="15">
-        <v>6688</v>
+        <v>668.8</v>
       </c>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
@@ -4262,7 +4262,7 @@
         <v>2125</v>
       </c>
       <c r="H75" s="15">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="I75" s="15"/>
       <c r="J75" s="15"/>
@@ -4334,7 +4334,7 @@
         <v>1293</v>
       </c>
       <c r="H78" s="15">
-        <v>3662</v>
+        <v>366.2</v>
       </c>
       <c r="I78" s="15"/>
       <c r="J78" s="15"/>
@@ -4356,7 +4356,7 @@
         <v>1758</v>
       </c>
       <c r="H79" s="15">
-        <v>4919</v>
+        <v>491.9</v>
       </c>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
@@ -4378,7 +4378,7 @@
         <v>1372</v>
       </c>
       <c r="H80" s="15">
-        <v>3949</v>
+        <v>394.9</v>
       </c>
       <c r="I80" s="15"/>
       <c r="J80" s="15"/>
@@ -4400,7 +4400,7 @@
         <v>1744</v>
       </c>
       <c r="H81" s="15">
-        <v>5019</v>
+        <v>501.9</v>
       </c>
       <c r="I81" s="15"/>
       <c r="J81" s="15"/>
@@ -4522,7 +4522,7 @@
         <v>1581</v>
       </c>
       <c r="H86" s="15">
-        <v>4927</v>
+        <v>492.7</v>
       </c>
       <c r="I86" s="15"/>
       <c r="J86" s="15"/>
@@ -4544,7 +4544,7 @@
         <v>1911</v>
       </c>
       <c r="H87" s="15">
-        <v>5940</v>
+        <v>594</v>
       </c>
       <c r="I87" s="15"/>
       <c r="J87" s="15"/>

</xml_diff>